<commit_message>
Importar productos desde excel incluyendo el codigo producto
</commit_message>
<xml_diff>
--- a/public/media/excel-import/Plantilla - Importar figuras.xlsx
+++ b/public/media/excel-import/Plantilla - Importar figuras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Baeza\Documents\kori\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904FE32D-C538-4DE8-A2A0-AC9D0364C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0A487C-1455-4D46-AA99-52A10BED09C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Q-Posket YUJI ITADORI B</t>
-  </si>
-  <si>
-    <t>Jujutsu Kaisen</t>
   </si>
   <si>
     <t>Kimetsu no Yaiba</t>
@@ -91,6 +88,21 @@
   </si>
   <si>
     <t>Dimensiones : 6.5 x 6.75 x 6.3 pulgadas</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>KORIQ4zChClzm</t>
+  </si>
+  <si>
+    <t>Jujutsu Kaisen;juan</t>
+  </si>
+  <si>
+    <t>KORIS5zZjCqzn</t>
   </si>
 </sst>
 </file>
@@ -439,119 +451,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2">
+        <v>23000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2">
-        <v>23000</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D4" s="2">
+        <v>70000</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2">
-        <v>30000</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2">
-        <v>70000</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>